<commit_message>
Updated Project Plan aproved by Talha
</commit_message>
<xml_diff>
--- a/Project Plan/Project Plan.xlsx
+++ b/Project Plan/Project Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitaliy\SkyDrive\School\Year 4\Capstone 4ZP6\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitaliy\Documents\GitHub\Porter-Simulation\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,15 +15,15 @@
     <sheet name="Detailed Workplan" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Detailed Workplan'!$A$1:$J$57</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Detailed Workplan'!$14:$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Detailed Workplan'!$A$1:$J$60</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Detailed Workplan'!$14:$18</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
   <si>
     <t>Complete</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Students deliver a demonstration for the course</t>
   </si>
   <si>
-    <t>6,5</t>
-  </si>
-  <si>
     <t>Develop final version of the product</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>Revision 1 Final Documentation</t>
   </si>
   <si>
-    <t>14,15</t>
-  </si>
-  <si>
     <t>Students create the first version of the user manual for the course</t>
   </si>
   <si>
@@ -202,9 +196,6 @@
     <t>set up a meeting sometime during this period</t>
   </si>
   <si>
-    <t>13,14,15,16</t>
-  </si>
-  <si>
     <t>Lead usability tests with users of the product</t>
   </si>
   <si>
@@ -227,6 +218,21 @@
   </si>
   <si>
     <t>Software Documentation</t>
+  </si>
+  <si>
+    <t>Discuss scope with HHS</t>
+  </si>
+  <si>
+    <t>HHS/Students</t>
+  </si>
+  <si>
+    <t>hold a meeting to  discuss current scope and overall delivery</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Talha will coordinate bi-weekly meetings to discuss current progress</t>
   </si>
 </sst>
 </file>
@@ -460,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -619,6 +625,12 @@
     <xf numFmtId="15" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,11 +655,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,67 +783,70 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Detailed Workplan'!$C$18:$C$37</c:f>
+              <c:f>'Detailed Workplan'!$C$20:$C$40</c:f>
               <c:strCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Revision 0 of the design documentation to be completed by students for the course</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Discuss scope with HHS</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Receive sample data from HHS</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Develop proof on concept version based on current requirements, and sample data</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Deliver first demo to HHS representatives</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Students deliver a demonstration for the course</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Receive feedback from HHS</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Meet withh HHS representatives to discuss feedback and additional requirements, if any</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Develop final version of the product</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Students create the first version of the user manual for the course</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Student deliver a first version of the test results for the software for the course</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Deliver second demo of the product to HHS staff</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Receive final feedback from HHS</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>If possible, apply minor changes according to feedback</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Develop software design documentation + user manual</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Lead usability tests with users of the product</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Perform scenario/stress tests on final product</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Capstone Milestone</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Capstone Milestone</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Capstone Milestone</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Provide final project report + design documentation + user manual + Final Demonstration</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Install final version of software on department computers</c:v>
                 </c:pt>
               </c:strCache>
@@ -832,42 +854,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Detailed Workplan'!$F$18:$F$37</c:f>
+              <c:f>'Detailed Workplan'!$F$20:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>41645</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>41652</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41653</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>41645</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>41645</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>41666</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>41653</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>41670</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>41678</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>41685</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>41677</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>41688</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41715</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>41715</c:v>
@@ -876,24 +898,27 @@
                   <c:v>41715</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>41715</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>41645</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41722</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>41722</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41702</c:v>
+                  <c:v>41722</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>41702</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>41702</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>41743</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>41743</c:v>
                 </c:pt>
               </c:numCache>
@@ -918,67 +943,70 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Detailed Workplan'!$C$18:$C$37</c:f>
+              <c:f>'Detailed Workplan'!$C$20:$C$40</c:f>
               <c:strCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Revision 0 of the design documentation to be completed by students for the course</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Discuss scope with HHS</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Receive sample data from HHS</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Develop proof on concept version based on current requirements, and sample data</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Deliver first demo to HHS representatives</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Students deliver a demonstration for the course</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Receive feedback from HHS</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Meet withh HHS representatives to discuss feedback and additional requirements, if any</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Develop final version of the product</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Students create the first version of the user manual for the course</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Student deliver a first version of the test results for the software for the course</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Deliver second demo of the product to HHS staff</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Receive final feedback from HHS</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>If possible, apply minor changes according to feedback</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Develop software design documentation + user manual</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Lead usability tests with users of the product</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Perform scenario/stress tests on final product</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Capstone Milestone</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Capstone Milestone</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Capstone Milestone</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Provide final project report + design documentation + user manual + Final Demonstration</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Install final version of software on department computers</c:v>
                 </c:pt>
               </c:strCache>
@@ -986,68 +1014,71 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Detailed Workplan'!$H$18:$H$37</c:f>
+              <c:f>'Detailed Workplan'!$H$20:$H$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -1064,11 +1095,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-116858928"/>
-        <c:axId val="-116864912"/>
+        <c:axId val="-955061392"/>
+        <c:axId val="-955058672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-116858928"/>
+        <c:axId val="-955061392"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1111,7 +1142,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-116864912"/>
+        <c:crossAx val="-955058672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1119,7 +1150,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-116864912"/>
+        <c:axId val="-955058672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="41747"/>
@@ -1172,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-116858928"/>
+        <c:crossAx val="-955061392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -1841,13 +1872,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>87084</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>136070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>2808514</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>54428</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2218,10 +2249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J334"/>
+  <dimension ref="A1:J337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -2238,7 +2269,7 @@
     <col min="15" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="7" t="s">
@@ -2251,7 +2282,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="1:10" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="17"/>
@@ -2262,14 +2293,14 @@
       <c r="H2" s="20"/>
       <c r="I2" s="21"/>
     </row>
-    <row r="3" spans="1:10" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="65" t="s">
+    <row r="3" spans="1:9" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="69"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -2277,10 +2308,10 @@
       <c r="H3" s="20"/>
       <c r="I3" s="21"/>
     </row>
-    <row r="4" spans="1:10" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
+    <row r="4" spans="1:9" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="67"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
@@ -2288,10 +2319,10 @@
       <c r="H4" s="20"/>
       <c r="I4" s="21"/>
     </row>
-    <row r="5" spans="1:10" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+    <row r="5" spans="1:9" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="67"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
@@ -2299,10 +2330,10 @@
       <c r="H5" s="20"/>
       <c r="I5" s="21"/>
     </row>
-    <row r="6" spans="1:10" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+    <row r="6" spans="1:9" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="67"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -2310,14 +2341,14 @@
       <c r="H6" s="20"/>
       <c r="I6" s="21"/>
     </row>
-    <row r="7" spans="1:10" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="70">
-        <v>1</v>
-      </c>
-      <c r="C7" s="71"/>
+      <c r="B7" s="72">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C7" s="73"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -2325,827 +2356,861 @@
       <c r="H7" s="20"/>
       <c r="I7" s="21"/>
     </row>
-    <row r="8" spans="1:10" s="18" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+    <row r="8" spans="1:9" s="18" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="1:10" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A9" s="41"/>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="64"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="48"/>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="64"/>
-    </row>
-    <row r="10" spans="1:10" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="F9" s="66"/>
+    </row>
+    <row r="10" spans="1:9" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="64"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="50"/>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="64"/>
-    </row>
-    <row r="11" spans="1:10" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="F10" s="66"/>
+    </row>
+    <row r="11" spans="1:9" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="64"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="51"/>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="64"/>
-    </row>
-    <row r="12" spans="1:10" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="F11" s="66"/>
+    </row>
+    <row r="12" spans="1:9" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="64"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="48"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-    </row>
-    <row r="13" spans="1:10" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+    </row>
+    <row r="13" spans="1:9" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="64"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="48"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-    </row>
-    <row r="14" spans="1:10" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+    </row>
+    <row r="14" spans="1:9" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A14" s="45"/>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="64"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="48"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-    </row>
-    <row r="15" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+    </row>
+    <row r="15" spans="1:9" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="1:10" s="24" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+    </row>
+    <row r="16" spans="1:9" s="18" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A16" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+    </row>
+    <row r="17" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="19"/>
+    </row>
+    <row r="18" spans="1:10" s="24" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B18" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C18" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D18" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E18" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F18" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="32" t="s">
+      <c r="H18" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="40" t="s">
+      <c r="J18" s="40" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="24" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
+    <row r="19" spans="1:10" s="24" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="68"/>
-    </row>
-    <row r="18" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="53" t="s">
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="70"/>
+    </row>
+    <row r="20" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="46">
+      <c r="B20" s="46">
         <v>1</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C20" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D20" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E20" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F20" s="52">
         <v>41645</v>
       </c>
-      <c r="G18" s="52">
+      <c r="G20" s="52">
         <v>41653</v>
       </c>
-      <c r="H18" s="46">
-        <f>G18-F18</f>
+      <c r="H20" s="46">
+        <f>G20-F20</f>
         <v>8</v>
       </c>
-      <c r="I18" s="56"/>
-      <c r="J18" s="72"/>
-    </row>
-    <row r="19" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="46">
-        <v>2</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="52">
-        <v>41645</v>
-      </c>
-      <c r="G19" s="52">
-        <v>41652</v>
-      </c>
-      <c r="H19" s="46">
-        <f t="shared" ref="H19:H35" si="0">G19-F19</f>
-        <v>7</v>
-      </c>
-      <c r="I19" s="56"/>
-      <c r="J19" s="73" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="46">
-        <v>3</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="32">
-        <v>2</v>
-      </c>
-      <c r="F20" s="54">
-        <v>41645</v>
-      </c>
-      <c r="G20" s="54">
-        <v>41663</v>
-      </c>
-      <c r="H20" s="46">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="I20" s="57"/>
-      <c r="J20" s="26"/>
-    </row>
-    <row r="21" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="56"/>
+      <c r="J20" s="64"/>
+    </row>
+    <row r="21" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="55" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="46">
-        <v>4</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="32">
-        <v>3</v>
-      </c>
-      <c r="F21" s="54">
-        <v>41666</v>
-      </c>
-      <c r="G21" s="54">
-        <v>41670</v>
+        <v>2</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="52">
+        <v>41652</v>
+      </c>
+      <c r="G21" s="52">
+        <v>41663</v>
       </c>
       <c r="H21" s="46">
         <f>G21-F21</f>
-        <v>4</v>
-      </c>
-      <c r="I21" s="58"/>
-      <c r="J21" s="26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="53" t="s">
-        <v>37</v>
+        <v>11</v>
+      </c>
+      <c r="I21" s="56"/>
+      <c r="J21" s="65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="55" t="s">
+        <v>14</v>
       </c>
       <c r="B22" s="46">
-        <v>5</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="31">
+        <f>B21</f>
+        <v>2</v>
+      </c>
+      <c r="F22" s="52">
+        <v>41653</v>
+      </c>
+      <c r="G22" s="52">
+        <v>41663</v>
+      </c>
+      <c r="H22" s="46">
+        <f>G22-F22</f>
         <v>10</v>
       </c>
-      <c r="E22" s="32">
-        <v>1</v>
-      </c>
-      <c r="F22" s="54">
-        <v>41653</v>
-      </c>
-      <c r="G22" s="54">
-        <v>41677</v>
-      </c>
-      <c r="H22" s="46">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="I22" s="58"/>
-      <c r="J22" s="26"/>
-    </row>
-    <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I22" s="56"/>
+      <c r="J22" s="65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="55" t="s">
         <v>14</v>
       </c>
       <c r="B23" s="46">
-        <v>6</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E23" s="32">
-        <v>4</v>
+        <f>B22</f>
+        <v>3</v>
       </c>
       <c r="F23" s="54">
-        <v>41670</v>
+        <v>41645</v>
       </c>
       <c r="G23" s="54">
-        <v>41677</v>
+        <v>41663</v>
       </c>
       <c r="H23" s="46">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f t="shared" ref="H23:H38" si="0">G23-F23</f>
+        <v>18</v>
       </c>
       <c r="I23" s="57"/>
-      <c r="J23" s="26" t="s">
-        <v>57</v>
-      </c>
+      <c r="J23" s="26"/>
     </row>
     <row r="24" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="55" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="46">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="32" t="s">
-        <v>39</v>
+      <c r="E24" s="32">
+        <f>B23</f>
+        <v>4</v>
       </c>
       <c r="F24" s="54">
+        <v>41666</v>
+      </c>
+      <c r="G24" s="54">
+        <v>41670</v>
+      </c>
+      <c r="H24" s="46">
+        <f>G24-F24</f>
+        <v>4</v>
+      </c>
+      <c r="I24" s="58"/>
+      <c r="J24" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="46">
+        <v>6</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="32">
+        <f>B20</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="54">
+        <v>41653</v>
+      </c>
+      <c r="G25" s="54">
+        <v>41677</v>
+      </c>
+      <c r="H25" s="46">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="I25" s="58"/>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A26" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="46">
+        <v>7</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="32">
+        <f>B24</f>
+        <v>5</v>
+      </c>
+      <c r="F26" s="54">
+        <v>41670</v>
+      </c>
+      <c r="G26" s="54">
+        <v>41677</v>
+      </c>
+      <c r="H26" s="46">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I26" s="57"/>
+      <c r="J26" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="46">
+        <v>8</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="32" t="str">
+        <f>CONCATENATE(B25,",",B26)</f>
+        <v>6,7</v>
+      </c>
+      <c r="F27" s="54">
         <v>41678</v>
       </c>
-      <c r="G24" s="62">
+      <c r="G27" s="62">
         <v>41684</v>
       </c>
-      <c r="H24" s="46">
+      <c r="H27" s="46">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I24" s="59"/>
-      <c r="J24" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A25" s="55" t="s">
+      <c r="I27" s="59"/>
+      <c r="J27" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A28" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="46">
+      <c r="B28" s="46">
+        <v>9</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="33">
+        <f>B27</f>
         <v>8</v>
       </c>
-      <c r="C25" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="33" t="s">
+      <c r="F28" s="35">
+        <v>41685</v>
+      </c>
+      <c r="G28" s="35">
+        <v>41715</v>
+      </c>
+      <c r="H28" s="46">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I28" s="59"/>
+      <c r="J28" s="28"/>
+    </row>
+    <row r="29" spans="1:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="46">
         <v>10</v>
       </c>
-      <c r="E25" s="33">
-        <v>7</v>
-      </c>
-      <c r="F25" s="35">
-        <v>41685</v>
-      </c>
-      <c r="G25" s="35">
-        <v>41722</v>
-      </c>
-      <c r="H25" s="46">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="I25" s="59"/>
-      <c r="J25" s="28"/>
-    </row>
-    <row r="26" spans="1:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="33">
-        <v>9</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="38" t="s">
+      <c r="C29" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="38">
-        <v>5</v>
-      </c>
-      <c r="F26" s="63">
+      <c r="E29" s="38">
+        <f>B25</f>
+        <v>6</v>
+      </c>
+      <c r="F29" s="63">
         <v>41677</v>
       </c>
-      <c r="G26" s="63">
+      <c r="G29" s="63">
         <v>41688</v>
       </c>
-      <c r="H26" s="46">
+      <c r="H29" s="46">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="I26" s="59"/>
-      <c r="J26" s="37"/>
-    </row>
-    <row r="27" spans="1:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="33">
+      <c r="I29" s="59"/>
+      <c r="J29" s="37"/>
+    </row>
+    <row r="30" spans="1:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="46">
+        <v>11</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="38" t="s">
+      <c r="E30" s="38">
+        <f>B29</f>
         <v>10</v>
       </c>
-      <c r="E27" s="38">
-        <v>9</v>
-      </c>
-      <c r="F27" s="63">
+      <c r="F30" s="63">
         <v>41688</v>
       </c>
-      <c r="G27" s="63">
+      <c r="G30" s="63">
         <v>41702</v>
       </c>
-      <c r="H27" s="46">
+      <c r="H30" s="46">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="I27" s="61"/>
-      <c r="J27" s="37"/>
-    </row>
-    <row r="28" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="55" t="s">
+      <c r="I30" s="61"/>
+      <c r="J30" s="37"/>
+    </row>
+    <row r="31" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="33">
-        <v>11</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="30" t="s">
+      <c r="B31" s="46">
+        <v>12</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="30">
-        <v>8</v>
-      </c>
-      <c r="F28" s="35">
+      <c r="E31" s="30">
+        <f>B28</f>
+        <v>9</v>
+      </c>
+      <c r="F31" s="35">
         <v>41715</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G31" s="35">
         <v>41719</v>
       </c>
-      <c r="H28" s="46">
+      <c r="H31" s="46">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I28" s="59"/>
-      <c r="J28" s="29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="55" t="s">
+      <c r="I31" s="59"/>
+      <c r="J31" s="29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="33">
+      <c r="B32" s="46">
+        <v>13</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="33">
+        <f>B31</f>
         <v>12</v>
       </c>
-      <c r="C29" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="33">
-        <v>11</v>
-      </c>
-      <c r="F29" s="35">
+      <c r="F32" s="35">
         <v>41715</v>
       </c>
-      <c r="G29" s="62">
+      <c r="G32" s="62">
         <v>41722</v>
       </c>
-      <c r="H29" s="46">
+      <c r="H32" s="46">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I29" s="59"/>
-      <c r="J29" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="38.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="55" t="s">
+      <c r="I32" s="59"/>
+      <c r="J32" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="38.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="33">
+      <c r="B33" s="46">
+        <v>14</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="33">
+        <f>B32</f>
         <v>13</v>
       </c>
-      <c r="C30" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="33">
-        <v>12</v>
-      </c>
-      <c r="F30" s="35">
+      <c r="F33" s="35">
         <v>41715</v>
       </c>
-      <c r="G30" s="35">
+      <c r="G33" s="35">
         <v>41722</v>
       </c>
-      <c r="H30" s="46">
+      <c r="H33" s="46">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I30" s="59"/>
-      <c r="J30" s="36"/>
-    </row>
-    <row r="31" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="33">
-        <v>14</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="38" t="s">
+      <c r="I33" s="59"/>
+      <c r="J33" s="36"/>
+    </row>
+    <row r="34" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="46">
+        <v>15</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="38">
-        <v>7</v>
-      </c>
-      <c r="F31" s="63">
+      <c r="E34" s="38">
+        <f>B27</f>
+        <v>8</v>
+      </c>
+      <c r="F34" s="63">
         <v>41645</v>
       </c>
-      <c r="G31" s="63">
+      <c r="G34" s="63">
         <v>41722</v>
       </c>
-      <c r="H31" s="46">
+      <c r="H34" s="46">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="I31" s="59"/>
-      <c r="J31" s="37"/>
-    </row>
-    <row r="32" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="55" t="s">
+      <c r="I34" s="59"/>
+      <c r="J34" s="37"/>
+    </row>
+    <row r="35" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="33">
-        <v>15</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="33" t="s">
+      <c r="B35" s="46">
+        <v>16</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="33">
-        <v>12</v>
-      </c>
-      <c r="F32" s="35">
+      <c r="E35" s="33">
+        <f>B32</f>
+        <v>13</v>
+      </c>
+      <c r="F35" s="35">
         <v>41722</v>
       </c>
-      <c r="G32" s="35">
+      <c r="G35" s="35">
         <v>41726</v>
       </c>
-      <c r="H32" s="46">
+      <c r="H35" s="46">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I32" s="60"/>
-      <c r="J32" s="28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="55" t="s">
+      <c r="I35" s="60"/>
+      <c r="J35" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="33">
-        <v>16</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="38" t="s">
+      <c r="B36" s="46">
+        <v>17</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="38">
-        <v>12</v>
-      </c>
-      <c r="F33" s="35">
+      <c r="E36" s="38">
+        <f>B32</f>
+        <v>13</v>
+      </c>
+      <c r="F36" s="35">
         <v>41722</v>
       </c>
-      <c r="G33" s="35">
+      <c r="G36" s="35">
         <v>41726</v>
       </c>
-      <c r="H33" s="46">
+      <c r="H36" s="46">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I33" s="61"/>
-      <c r="J33" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A34" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="33">
-        <v>17</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="33" t="s">
+      <c r="I36" s="61"/>
+      <c r="J36" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A37" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="46">
+        <v>18</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="33">
-        <v>10</v>
-      </c>
-      <c r="F34" s="35">
+      <c r="E37" s="33">
+        <f>B30</f>
+        <v>11</v>
+      </c>
+      <c r="F37" s="35">
         <v>41702</v>
       </c>
-      <c r="G34" s="35">
+      <c r="G37" s="35">
         <v>41728</v>
       </c>
-      <c r="H34" s="46">
+      <c r="H37" s="46">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="I34" s="57"/>
-      <c r="J34" s="39"/>
-    </row>
-    <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A35" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="33">
-        <v>18</v>
-      </c>
-      <c r="C35" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D35" s="33" t="s">
+      <c r="I37" s="57"/>
+      <c r="J37" s="39"/>
+    </row>
+    <row r="38" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A38" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="46">
+        <v>19</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="33">
-        <v>10</v>
-      </c>
-      <c r="F35" s="35">
+      <c r="E38" s="33">
+        <f>B30</f>
+        <v>11</v>
+      </c>
+      <c r="F38" s="35">
         <v>41702</v>
       </c>
-      <c r="G35" s="35">
+      <c r="G38" s="35">
         <v>41728</v>
       </c>
-      <c r="H35" s="46">
+      <c r="H38" s="46">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="I35" s="57"/>
-      <c r="J35" s="39"/>
-    </row>
-    <row r="36" spans="1:10" ht="34.200000000000003" x14ac:dyDescent="0.2">
-      <c r="A36" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="33">
-        <v>19</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="33" t="s">
+      <c r="I38" s="57"/>
+      <c r="J38" s="39"/>
+    </row>
+    <row r="39" spans="1:10" ht="34.200000000000003" x14ac:dyDescent="0.2">
+      <c r="A39" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="46">
+        <v>20</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="F36" s="35">
+      <c r="E39" s="33" t="str">
+        <f>CONCATENATE(B33,",",B34,",",B35,",",B36)</f>
+        <v>14,15,16,17</v>
+      </c>
+      <c r="F39" s="35">
         <v>41743</v>
       </c>
-      <c r="G36" s="35">
+      <c r="G39" s="35">
         <v>41747</v>
       </c>
-      <c r="H36" s="46">
-        <f>G36-F36</f>
+      <c r="H39" s="46">
+        <f>G39-F39</f>
         <v>4</v>
       </c>
-      <c r="I36" s="57"/>
-      <c r="J36" s="39"/>
-    </row>
-    <row r="37" spans="1:10" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A37" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="33">
-        <v>20</v>
-      </c>
-      <c r="C37" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="33" t="s">
+      <c r="I39" s="57"/>
+      <c r="J39" s="39"/>
+    </row>
+    <row r="40" spans="1:10" ht="22.8" x14ac:dyDescent="0.2">
+      <c r="A40" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="46">
+        <v>21</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" s="35">
+      <c r="E40" s="33" t="str">
+        <f>CONCATENATE(B34,",",B35)</f>
+        <v>15,16</v>
+      </c>
+      <c r="F40" s="35">
         <v>41743</v>
       </c>
-      <c r="G37" s="35">
+      <c r="G40" s="35">
         <v>41747</v>
       </c>
-      <c r="H37" s="46">
-        <f>G37-F37</f>
+      <c r="H40" s="46">
+        <f>G40-F40</f>
         <v>4</v>
       </c>
-      <c r="I37" s="59"/>
-      <c r="J37" s="29"/>
-    </row>
-    <row r="38" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="8"/>
-    </row>
-    <row r="39" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="29"/>
+    </row>
+    <row r="41" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="14"/>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="9"/>
+    <row r="42" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="8"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="16"/>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="9"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="8"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
-      <c r="J44" s="9"/>
+      <c r="J44" s="8"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
@@ -3155,9 +3220,9 @@
       <c r="J45" s="9"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
@@ -3167,9 +3232,9 @@
       <c r="J46" s="9"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
@@ -3179,9 +3244,9 @@
       <c r="J47" s="9"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="10"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
@@ -3191,9 +3256,9 @@
       <c r="J48" s="9"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="10"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -3203,9 +3268,9 @@
       <c r="J49" s="9"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="10"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
@@ -3731,8 +3796,8 @@
       <c r="J93" s="9"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" s="9"/>
-      <c r="B94" s="9"/>
+      <c r="A94" s="12"/>
+      <c r="B94" s="12"/>
       <c r="C94" s="10"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
@@ -3743,8 +3808,8 @@
       <c r="J94" s="9"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
+      <c r="A95" s="12"/>
+      <c r="B95" s="12"/>
       <c r="C95" s="10"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
@@ -3755,8 +3820,8 @@
       <c r="J95" s="9"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
+      <c r="A96" s="12"/>
+      <c r="B96" s="12"/>
       <c r="C96" s="10"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
@@ -6622,10 +6687,49 @@
       <c r="I334" s="13"/>
       <c r="J334" s="9"/>
     </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A335" s="9"/>
+      <c r="B335" s="9"/>
+      <c r="C335" s="10"/>
+      <c r="D335" s="13"/>
+      <c r="E335" s="13"/>
+      <c r="F335" s="13"/>
+      <c r="G335" s="13"/>
+      <c r="H335" s="13"/>
+      <c r="I335" s="13"/>
+      <c r="J335" s="9"/>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A336" s="9"/>
+      <c r="B336" s="9"/>
+      <c r="C336" s="10"/>
+      <c r="D336" s="13"/>
+      <c r="E336" s="13"/>
+      <c r="F336" s="13"/>
+      <c r="G336" s="13"/>
+      <c r="H336" s="13"/>
+      <c r="I336" s="13"/>
+      <c r="J336" s="9"/>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A337" s="9"/>
+      <c r="B337" s="9"/>
+      <c r="C337" s="10"/>
+      <c r="D337" s="13"/>
+      <c r="E337" s="13"/>
+      <c r="F337" s="13"/>
+      <c r="G337" s="13"/>
+      <c r="H337" s="13"/>
+      <c r="I337" s="13"/>
+      <c r="J337" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A19:J19"/>
     <mergeCell ref="B3:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
@@ -6639,8 +6743,6 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.37" bottom="0.42" header="0.24" footer="0.24"/>

</xml_diff>